<commit_message>
Added Gracefull exit handlers
</commit_message>
<xml_diff>
--- a/docs/Formulas.xlsx
+++ b/docs/Formulas.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lauki\Documents\Git\redis-lsm-timeseries\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laukikragji/Documents/Git/Personal/redis-lsm-timeseries/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7A2F2E-15E6-4800-B6D9-6E1D1A654662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF39C06-FF7B-354F-A928-08247976DA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2868" yWindow="4704" windowWidth="17280" windowHeight="8964" xr2:uid="{5C38A616-3E13-4B6E-8DD4-4DE4002EE992}"/>
+    <workbookView xWindow="8180" yWindow="5400" windowWidth="17280" windowHeight="8960" activeTab="1" xr2:uid="{5C38A616-3E13-4B6E-8DD4-4DE4002EE992}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>TagId</t>
   </si>
@@ -37,6 +47,18 @@
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>Active threads</t>
+  </si>
+  <si>
+    <t>Response Time</t>
+  </si>
+  <si>
+    <t>TPS</t>
+  </si>
+  <si>
+    <t>Response time goes beyond 2000&gt; or we encounter error</t>
   </si>
 </sst>
 </file>
@@ -399,16 +421,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C73E7E-B446-47BB-BF22-4B051FF5EBFB}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -416,7 +438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -453,7 +475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -473,7 +495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -493,7 +515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -513,7 +535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -533,7 +555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -557,4 +579,50 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4ED677-F3F7-D949-9433-68F66723928D}">
+  <dimension ref="A2:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <f>(B2*1000)/B3</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>